<commit_message>
feat: add dashboard analytics with charts and statistics
- Added new /admin/api/analytics endpoint to fetch analytics data
  * Total downloads count
  * Unique students count
  * Peak hour analysis
  * Certificates by type breakdown
  * Top 5 students by download count
  * 30-day download trend

- Updated admin dashboard template with:
  * New Analytics tab with statistics cards
  * Doughnut chart for certificate type distribution
  * Bar chart for top 5 students
  * Line chart for 30-day download trends
  * Tab-based navigation between Analytics and Logs

- Added Chart.js library (v3.9.1) for visualizations
- Responsive grid layout for statistics cards
- Real-time data loading via AJAX
</commit_message>
<xml_diff>
--- a/student_certificates.xlsx
+++ b/student_certificates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X12"/>
+  <dimension ref="A1:X14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1571,6 +1571,82 @@
       <c r="W12" t="inlineStr"/>
       <c r="X12" t="inlineStr"/>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>HT2025EX</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Demo Student</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>STUDYING</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>TEST002</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Test2</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>